<commit_message>
EPBDS-11426 Not all java syntax formats are supported for Parameter types in Rules tables
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11337_NPE_DTConditionParamDefinedWithError.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11337_NPE_DTConditionParamDefinedWithError.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\demo\openl-demo\user-workspace\DEFAULT\NPEbug1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37A5F0B-96C6-4460-B857-56873D63A367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40C725F-EA7B-4E7B-8E1A-7E312A0F952C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="675" windowWidth="27360" windowHeight="15090" xr2:uid="{D2C7576E-0238-4E2B-8134-3BFA64FEF82E}"/>
+    <workbookView xWindow="3045" yWindow="855" windowWidth="21225" windowHeight="13500" xr2:uid="{D2C7576E-0238-4E2B-8134-3BFA64FEF82E}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -44,9 +39,6 @@
     <t>100, 200, 300</t>
   </si>
   <si>
-    <t>Integer [] intArr</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
@@ -54,6 +46,9 @@
   </si>
   <si>
     <t>Rules  Double mytest(Integer param1)</t>
+  </si>
+  <si>
+    <t>Integer [1] intArr</t>
   </si>
 </sst>
 </file>
@@ -111,10 +106,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -432,7 +427,7 @@
   <dimension ref="C3:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D9"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,52 +436,52 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>30</v>
       </c>
     </row>

</xml_diff>